<commit_message>
major update: add colum to database
</commit_message>
<xml_diff>
--- a/traffic_data.xlsx
+++ b/traffic_data.xlsx
@@ -17,6 +17,9 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="16">
   <si>
+    <t>pengguna</t>
+  </si>
+  <si>
     <t>Interval</t>
   </si>
   <si>
@@ -38,31 +41,28 @@
     <t>TB</t>
   </si>
   <si>
-    <t>3/11/2024 , 15:51:01 - 15:51:06</t>
+    <t>3/13/2024 , 12:12:09 - 12:12:14</t>
   </si>
   <si>
     <t>0 Menit 5 Detik</t>
   </si>
   <si>
-    <t>3/11/2024 , 15:51:10 - 15:51:12</t>
-  </si>
-  <si>
-    <t>0 Menit 2 Detik</t>
-  </si>
-  <si>
-    <t>3/11/2024 , 16:01:40 - 16:01:45</t>
-  </si>
-  <si>
-    <t>3/11/2024 , 19:32:11 - 19:32:16</t>
-  </si>
-  <si>
-    <t>3/11/2024 , 19:32:28 - 19:32:31</t>
+    <t>wiki</t>
+  </si>
+  <si>
+    <t>3/13/2024 , 12:55:30 - 12:55:33</t>
   </si>
   <si>
     <t>0 Menit 3 Detik</t>
   </si>
   <si>
-    <t>3/11/2024 , 20:35:37 - 20:35:39</t>
+    <t>mikhael</t>
+  </si>
+  <si>
+    <t>3/13/2024 , 12:56:57 - 12:57:05</t>
+  </si>
+  <si>
+    <t>0 Menit 8 Detik</t>
   </si>
 </sst>
 </file>
@@ -402,7 +402,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -410,7 +410,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:8">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -432,143 +432,83 @@
       <c r="G1" t="s">
         <v>6</v>
       </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
     </row>
-    <row r="2" spans="1:7">
-      <c r="A2" t="s">
-        <v>7</v>
-      </c>
+    <row r="2" spans="1:8">
       <c r="B2" t="s">
         <v>8</v>
       </c>
-      <c r="C2">
-        <v>3</v>
+      <c r="C2" t="s">
+        <v>9</v>
       </c>
       <c r="D2">
         <v>2</v>
       </c>
       <c r="E2">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="F2">
+        <v>2</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="H2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3">
         <v>4</v>
       </c>
-      <c r="G2">
+      <c r="E3">
         <v>4</v>
       </c>
-    </row>
-    <row r="3" spans="1:7">
-      <c r="A3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3">
-        <v>3</v>
-      </c>
-      <c r="D3">
-        <v>2</v>
-      </c>
-      <c r="E3">
-        <v>5</v>
-      </c>
       <c r="F3">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="G3">
         <v>4</v>
       </c>
+      <c r="H3">
+        <v>31</v>
+      </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:8">
       <c r="A4" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4">
-        <v>0</v>
+        <v>14</v>
+      </c>
+      <c r="C4" t="s">
+        <v>15</v>
       </c>
       <c r="D4">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E4">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F4">
+        <v>2</v>
+      </c>
+      <c r="G4">
+        <v>3</v>
+      </c>
+      <c r="H4">
         <v>1</v>
-      </c>
-      <c r="G4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7">
-      <c r="A5" t="s">
-        <v>12</v>
-      </c>
-      <c r="B5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C5">
-        <v>10</v>
-      </c>
-      <c r="D5">
-        <v>10</v>
-      </c>
-      <c r="E5">
-        <v>10</v>
-      </c>
-      <c r="F5">
-        <v>10</v>
-      </c>
-      <c r="G5">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7">
-      <c r="A6" t="s">
-        <v>13</v>
-      </c>
-      <c r="B6" t="s">
-        <v>14</v>
-      </c>
-      <c r="C6">
-        <v>10</v>
-      </c>
-      <c r="D6">
-        <v>10</v>
-      </c>
-      <c r="E6">
-        <v>10</v>
-      </c>
-      <c r="F6">
-        <v>10</v>
-      </c>
-      <c r="G6">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7">
-      <c r="A7" t="s">
-        <v>15</v>
-      </c>
-      <c r="B7" t="s">
-        <v>10</v>
-      </c>
-      <c r="C7">
-        <v>10</v>
-      </c>
-      <c r="D7">
-        <v>10</v>
-      </c>
-      <c r="E7">
-        <v>10</v>
-      </c>
-      <c r="F7">
-        <v>10</v>
-      </c>
-      <c r="G7">
-        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
docs: update readme with project details and screenshots
</commit_message>
<xml_diff>
--- a/traffic_data.xlsx
+++ b/traffic_data.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="8">
   <si>
     <t>surveyor</t>
   </si>
@@ -39,36 +39,6 @@
   </si>
   <si>
     <t>TB</t>
-  </si>
-  <si>
-    <t>DEVELOPER</t>
-  </si>
-  <si>
-    <t>5/19/2024 , 13:09:59 - 13:10:01</t>
-  </si>
-  <si>
-    <t>0 Menit 2 Detik</t>
-  </si>
-  <si>
-    <t>5/19/2024 , 16:59:14 - 16:59:16</t>
-  </si>
-  <si>
-    <t>5/19/2024 , 16:59:36 - 16:59:37</t>
-  </si>
-  <si>
-    <t>0 Menit 1 Detik</t>
-  </si>
-  <si>
-    <t>5/19/2024 , 16:59:39 - 16:59:42</t>
-  </si>
-  <si>
-    <t>0 Menit 3 Detik</t>
-  </si>
-  <si>
-    <t>5/19/2024 , 17:02:15 - 17:02:18</t>
-  </si>
-  <si>
-    <t>5/21/2024 , 23:28:15 - 23:28:17</t>
   </si>
 </sst>
 </file>
@@ -408,7 +378,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:H7"/>
+  <dimension ref="A1:H1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -442,162 +412,6 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
-      <c r="A2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D2">
-        <v>0</v>
-      </c>
-      <c r="E2">
-        <v>0</v>
-      </c>
-      <c r="F2">
-        <v>0</v>
-      </c>
-      <c r="G2">
-        <v>1</v>
-      </c>
-      <c r="H2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8">
-      <c r="A3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3">
-        <v>0</v>
-      </c>
-      <c r="E3">
-        <v>0</v>
-      </c>
-      <c r="F3">
-        <v>0</v>
-      </c>
-      <c r="G3">
-        <v>0</v>
-      </c>
-      <c r="H3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8">
-      <c r="A4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D4">
-        <v>0</v>
-      </c>
-      <c r="E4">
-        <v>0</v>
-      </c>
-      <c r="F4">
-        <v>0</v>
-      </c>
-      <c r="G4">
-        <v>0</v>
-      </c>
-      <c r="H4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8">
-      <c r="A5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C5" t="s">
-        <v>15</v>
-      </c>
-      <c r="D5">
-        <v>0</v>
-      </c>
-      <c r="E5">
-        <v>0</v>
-      </c>
-      <c r="F5">
-        <v>0</v>
-      </c>
-      <c r="G5">
-        <v>0</v>
-      </c>
-      <c r="H5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8">
-      <c r="A6" t="s">
-        <v>8</v>
-      </c>
-      <c r="B6" t="s">
-        <v>16</v>
-      </c>
-      <c r="C6" t="s">
-        <v>15</v>
-      </c>
-      <c r="D6">
-        <v>0</v>
-      </c>
-      <c r="E6">
-        <v>0</v>
-      </c>
-      <c r="F6">
-        <v>0</v>
-      </c>
-      <c r="G6">
-        <v>0</v>
-      </c>
-      <c r="H6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8">
-      <c r="A7" t="s">
-        <v>8</v>
-      </c>
-      <c r="B7" t="s">
-        <v>17</v>
-      </c>
-      <c r="C7" t="s">
-        <v>10</v>
-      </c>
-      <c r="D7">
-        <v>0</v>
-      </c>
-      <c r="E7">
-        <v>0</v>
-      </c>
-      <c r="F7">
-        <v>0</v>
-      </c>
-      <c r="G7">
-        <v>0</v>
-      </c>
-      <c r="H7">
-        <v>0</v>
-      </c>
-    </row>
   </sheetData>
   <printOptions gridLines="false" gridLinesSet="true"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>